<commit_message>
EmailUtil changes, Login and session changes
</commit_message>
<xml_diff>
--- a/InventoryWeb/resources/PO_Template.xlsx
+++ b/InventoryWeb/resources/PO_Template.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Ceasefire-001" sheetId="46" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Ceasefire-001'!$A$4:$O$41</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Ceasefire-001'!$A$4:$O$35</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
   <extLst>
@@ -300,7 +300,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -742,6 +742,19 @@
       <top style="thin">
         <color auto="1"/>
       </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -893,7 +906,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="160">
+  <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1056,22 +1069,10 @@
     <xf numFmtId="2" fontId="5" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1098,14 +1099,17 @@
     <xf numFmtId="3" fontId="5" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1218,14 +1222,8 @@
     <xf numFmtId="3" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1256,27 +1254,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1347,26 +1324,29 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="140">
@@ -1530,13 +1510,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>434554</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>44026</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>397933</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>25399</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1574,13 +1554,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>67733</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>93135</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>518160</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>33867</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1939,10 +1919,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B8:P41"/>
+  <dimension ref="B8:P35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22:I22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26:I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1986,42 +1966,42 @@
       <c r="O9" s="49"/>
     </row>
     <row r="10" spans="2:15" s="2" customFormat="1" ht="18.600000000000001" customHeight="1">
-      <c r="B10" s="130" t="s">
+      <c r="B10" s="118" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="131"/>
-      <c r="D10" s="131"/>
-      <c r="E10" s="131"/>
-      <c r="F10" s="131"/>
-      <c r="G10" s="131"/>
-      <c r="H10" s="132"/>
-      <c r="I10" s="133" t="s">
+      <c r="C10" s="119"/>
+      <c r="D10" s="119"/>
+      <c r="E10" s="119"/>
+      <c r="F10" s="119"/>
+      <c r="G10" s="119"/>
+      <c r="H10" s="120"/>
+      <c r="I10" s="121" t="s">
         <v>2</v>
       </c>
-      <c r="J10" s="134"/>
-      <c r="K10" s="134"/>
-      <c r="L10" s="134"/>
-      <c r="M10" s="134"/>
-      <c r="N10" s="134"/>
-      <c r="O10" s="135"/>
+      <c r="J10" s="122"/>
+      <c r="K10" s="122"/>
+      <c r="L10" s="122"/>
+      <c r="M10" s="122"/>
+      <c r="N10" s="122"/>
+      <c r="O10" s="123"/>
     </row>
     <row r="11" spans="2:15" s="3" customFormat="1" ht="12.75">
-      <c r="B11" s="136" t="s">
+      <c r="B11" s="124" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="137"/>
-      <c r="D11" s="137"/>
-      <c r="E11" s="137"/>
-      <c r="F11" s="137"/>
-      <c r="G11" s="137"/>
-      <c r="H11" s="137"/>
-      <c r="I11" s="137"/>
-      <c r="J11" s="137"/>
-      <c r="K11" s="137"/>
-      <c r="L11" s="137"/>
-      <c r="M11" s="137"/>
-      <c r="N11" s="137"/>
-      <c r="O11" s="138"/>
+      <c r="C11" s="125"/>
+      <c r="D11" s="125"/>
+      <c r="E11" s="125"/>
+      <c r="F11" s="125"/>
+      <c r="G11" s="125"/>
+      <c r="H11" s="125"/>
+      <c r="I11" s="125"/>
+      <c r="J11" s="125"/>
+      <c r="K11" s="125"/>
+      <c r="L11" s="125"/>
+      <c r="M11" s="125"/>
+      <c r="N11" s="125"/>
+      <c r="O11" s="126"/>
     </row>
     <row r="12" spans="2:15" s="3" customFormat="1" ht="9.9499999999999993" customHeight="1">
       <c r="B12" s="32"/>
@@ -2040,121 +2020,121 @@
       <c r="O12" s="50"/>
     </row>
     <row r="13" spans="2:15">
-      <c r="B13" s="139" t="s">
+      <c r="B13" s="127" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="140"/>
-      <c r="D13" s="140" t="s">
+      <c r="C13" s="128"/>
+      <c r="D13" s="128" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="140"/>
-      <c r="F13" s="140"/>
-      <c r="G13" s="140"/>
+      <c r="E13" s="128"/>
+      <c r="F13" s="128"/>
+      <c r="G13" s="128"/>
       <c r="H13" s="23"/>
-      <c r="I13" s="141" t="s">
+      <c r="I13" s="129" t="s">
         <v>6</v>
       </c>
-      <c r="J13" s="142"/>
-      <c r="K13" s="143"/>
-      <c r="L13" s="143"/>
-      <c r="M13" s="143"/>
-      <c r="N13" s="143"/>
-      <c r="O13" s="144"/>
+      <c r="J13" s="130"/>
+      <c r="K13" s="131"/>
+      <c r="L13" s="131"/>
+      <c r="M13" s="131"/>
+      <c r="N13" s="131"/>
+      <c r="O13" s="132"/>
     </row>
     <row r="14" spans="2:15">
-      <c r="B14" s="147" t="s">
+      <c r="B14" s="135" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="148"/>
-      <c r="D14" s="148" t="s">
+      <c r="C14" s="136"/>
+      <c r="D14" s="136" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="148"/>
-      <c r="F14" s="148"/>
-      <c r="G14" s="148"/>
+      <c r="E14" s="136"/>
+      <c r="F14" s="136"/>
+      <c r="G14" s="136"/>
       <c r="H14" s="24"/>
-      <c r="I14" s="149" t="s">
+      <c r="I14" s="137" t="s">
         <v>9</v>
       </c>
-      <c r="J14" s="150"/>
-      <c r="K14" s="125"/>
-      <c r="L14" s="125"/>
-      <c r="M14" s="125"/>
-      <c r="N14" s="125"/>
-      <c r="O14" s="126"/>
+      <c r="J14" s="138"/>
+      <c r="K14" s="143"/>
+      <c r="L14" s="143"/>
+      <c r="M14" s="143"/>
+      <c r="N14" s="143"/>
+      <c r="O14" s="144"/>
     </row>
     <row r="15" spans="2:15" ht="12.95" customHeight="1">
       <c r="B15" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="114"/>
-      <c r="D15" s="114"/>
-      <c r="E15" s="114"/>
-      <c r="F15" s="114"/>
-      <c r="G15" s="114"/>
-      <c r="H15" s="114"/>
-      <c r="I15" s="127" t="s">
+      <c r="C15" s="109"/>
+      <c r="D15" s="109"/>
+      <c r="E15" s="109"/>
+      <c r="F15" s="109"/>
+      <c r="G15" s="109"/>
+      <c r="H15" s="109"/>
+      <c r="I15" s="145" t="s">
         <v>11</v>
       </c>
-      <c r="J15" s="128"/>
-      <c r="K15" s="128"/>
-      <c r="L15" s="128"/>
-      <c r="M15" s="128"/>
-      <c r="N15" s="128"/>
-      <c r="O15" s="129"/>
+      <c r="J15" s="146"/>
+      <c r="K15" s="146"/>
+      <c r="L15" s="146"/>
+      <c r="M15" s="146"/>
+      <c r="N15" s="146"/>
+      <c r="O15" s="147"/>
     </row>
     <row r="16" spans="2:15" s="7" customFormat="1" ht="12.95" customHeight="1">
-      <c r="B16" s="151"/>
-      <c r="C16" s="152"/>
-      <c r="D16" s="152"/>
-      <c r="E16" s="152"/>
-      <c r="F16" s="152"/>
-      <c r="G16" s="152"/>
-      <c r="H16" s="152"/>
+      <c r="B16" s="139"/>
+      <c r="C16" s="140"/>
+      <c r="D16" s="140"/>
+      <c r="E16" s="140"/>
+      <c r="F16" s="140"/>
+      <c r="G16" s="140"/>
+      <c r="H16" s="140"/>
       <c r="I16" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J16" s="123" t="s">
+      <c r="J16" s="141" t="s">
         <v>13</v>
       </c>
-      <c r="K16" s="123"/>
-      <c r="L16" s="123"/>
-      <c r="M16" s="123"/>
-      <c r="N16" s="123"/>
-      <c r="O16" s="124"/>
+      <c r="K16" s="141"/>
+      <c r="L16" s="141"/>
+      <c r="M16" s="141"/>
+      <c r="N16" s="141"/>
+      <c r="O16" s="142"/>
     </row>
     <row r="17" spans="2:16" s="7" customFormat="1" ht="12.95" customHeight="1">
-      <c r="B17" s="113" t="s">
+      <c r="B17" s="108" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="114"/>
+      <c r="C17" s="109"/>
       <c r="D17" s="8"/>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
-      <c r="G17" s="114"/>
-      <c r="H17" s="114"/>
+      <c r="G17" s="109"/>
+      <c r="H17" s="109"/>
       <c r="I17" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="J17" s="123">
+      <c r="J17" s="141">
         <v>9766669933</v>
       </c>
-      <c r="K17" s="123"/>
-      <c r="L17" s="123"/>
-      <c r="M17" s="123"/>
-      <c r="N17" s="123"/>
-      <c r="O17" s="124"/>
+      <c r="K17" s="141"/>
+      <c r="L17" s="141"/>
+      <c r="M17" s="141"/>
+      <c r="N17" s="141"/>
+      <c r="O17" s="142"/>
     </row>
     <row r="18" spans="2:16" s="7" customFormat="1" ht="12.95" customHeight="1">
-      <c r="B18" s="113" t="s">
+      <c r="B18" s="108" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="114"/>
-      <c r="D18" s="145"/>
-      <c r="E18" s="145"/>
-      <c r="F18" s="145"/>
-      <c r="G18" s="145"/>
-      <c r="H18" s="146"/>
+      <c r="C18" s="109"/>
+      <c r="D18" s="133"/>
+      <c r="E18" s="133"/>
+      <c r="F18" s="133"/>
+      <c r="G18" s="133"/>
+      <c r="H18" s="134"/>
       <c r="I18" s="6" t="s">
         <v>17</v>
       </c>
@@ -2168,10 +2148,10 @@
       <c r="O18" s="51"/>
     </row>
     <row r="19" spans="2:16" s="7" customFormat="1" ht="12.95" customHeight="1">
-      <c r="B19" s="113" t="s">
+      <c r="B19" s="108" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="114"/>
+      <c r="C19" s="109"/>
       <c r="D19" s="34"/>
       <c r="E19" s="34"/>
       <c r="F19" s="34"/>
@@ -2190,27 +2170,27 @@
       <c r="O19" s="51"/>
     </row>
     <row r="20" spans="2:16" s="3" customFormat="1" ht="12.95" customHeight="1">
-      <c r="B20" s="115" t="s">
+      <c r="B20" s="110" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="117" t="s">
+      <c r="C20" s="112" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="118"/>
-      <c r="E20" s="117" t="s">
+      <c r="D20" s="113"/>
+      <c r="E20" s="112" t="s">
         <v>22</v>
       </c>
-      <c r="F20" s="121"/>
-      <c r="G20" s="121"/>
-      <c r="H20" s="121"/>
-      <c r="I20" s="118"/>
-      <c r="J20" s="77" t="s">
+      <c r="F20" s="116"/>
+      <c r="G20" s="116"/>
+      <c r="H20" s="116"/>
+      <c r="I20" s="113"/>
+      <c r="J20" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="K20" s="77" t="s">
+      <c r="K20" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="L20" s="73" t="s">
+      <c r="L20" s="70" t="s">
         <v>42</v>
       </c>
       <c r="M20" s="45" t="s">
@@ -2219,173 +2199,173 @@
       <c r="N20" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="O20" s="75" t="s">
+      <c r="O20" s="72" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="21" spans="2:16" s="3" customFormat="1" ht="12.95" customHeight="1">
-      <c r="B21" s="116"/>
-      <c r="C21" s="119"/>
-      <c r="D21" s="120"/>
-      <c r="E21" s="119"/>
-      <c r="F21" s="122"/>
-      <c r="G21" s="122"/>
-      <c r="H21" s="122"/>
-      <c r="I21" s="120"/>
-      <c r="J21" s="78"/>
-      <c r="K21" s="78"/>
-      <c r="L21" s="74"/>
+      <c r="B21" s="111"/>
+      <c r="C21" s="114"/>
+      <c r="D21" s="115"/>
+      <c r="E21" s="114"/>
+      <c r="F21" s="117"/>
+      <c r="G21" s="117"/>
+      <c r="H21" s="117"/>
+      <c r="I21" s="115"/>
+      <c r="J21" s="75"/>
+      <c r="K21" s="75"/>
+      <c r="L21" s="71"/>
       <c r="M21" s="43">
         <v>0.09</v>
       </c>
       <c r="N21" s="10">
         <v>0.09</v>
       </c>
-      <c r="O21" s="76"/>
+      <c r="O21" s="73"/>
     </row>
     <row r="22" spans="2:16" s="3" customFormat="1" ht="12.95" customHeight="1">
-      <c r="B22" s="154"/>
-      <c r="C22" s="60"/>
-      <c r="D22" s="61"/>
-      <c r="E22" s="91"/>
-      <c r="F22" s="92"/>
-      <c r="G22" s="92"/>
-      <c r="H22" s="92"/>
-      <c r="I22" s="93"/>
-      <c r="J22" s="155"/>
-      <c r="K22" s="155"/>
-      <c r="L22" s="156"/>
-      <c r="M22" s="43"/>
-      <c r="N22" s="43"/>
-      <c r="O22" s="157"/>
+      <c r="B22" s="67"/>
+      <c r="C22" s="67"/>
+      <c r="D22" s="67"/>
+      <c r="E22" s="107"/>
+      <c r="F22" s="107"/>
+      <c r="G22" s="107"/>
+      <c r="H22" s="107"/>
+      <c r="I22" s="107"/>
+      <c r="J22" s="67"/>
+      <c r="K22" s="67"/>
+      <c r="L22" s="68"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="69"/>
     </row>
     <row r="23" spans="2:16" s="3" customFormat="1" ht="12.95" customHeight="1">
-      <c r="B23" s="155"/>
-      <c r="C23" s="60"/>
-      <c r="D23" s="61"/>
-      <c r="E23" s="94"/>
-      <c r="F23" s="95"/>
-      <c r="G23" s="95"/>
-      <c r="H23" s="95"/>
-      <c r="I23" s="96"/>
-      <c r="J23" s="155"/>
-      <c r="K23" s="155"/>
-      <c r="L23" s="156"/>
-      <c r="M23" s="43"/>
-      <c r="N23" s="43"/>
-      <c r="O23" s="157"/>
-    </row>
-    <row r="24" spans="2:16" s="3" customFormat="1" ht="12.95" customHeight="1">
-      <c r="B24" s="11"/>
-      <c r="C24" s="71"/>
-      <c r="D24" s="70"/>
-      <c r="E24" s="153"/>
-      <c r="F24" s="158"/>
-      <c r="G24" s="158"/>
-      <c r="H24" s="158"/>
-      <c r="I24" s="159"/>
+      <c r="B23" s="67"/>
+      <c r="C23" s="67"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="107"/>
+      <c r="F23" s="107"/>
+      <c r="G23" s="107"/>
+      <c r="H23" s="107"/>
+      <c r="I23" s="107"/>
+      <c r="J23" s="67"/>
+      <c r="K23" s="67"/>
+      <c r="L23" s="68"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="69"/>
+    </row>
+    <row r="24" spans="2:16" s="3" customFormat="1" ht="12.75" customHeight="1">
+      <c r="B24" s="35"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="101"/>
+      <c r="F24" s="102"/>
+      <c r="G24" s="102"/>
+      <c r="H24" s="102"/>
+      <c r="I24" s="103"/>
       <c r="J24" s="11"/>
-      <c r="K24" s="11"/>
-      <c r="L24" s="72"/>
-      <c r="M24" s="43"/>
-      <c r="N24" s="43"/>
-      <c r="O24" s="55"/>
-    </row>
-    <row r="25" spans="2:16" s="3" customFormat="1" ht="12.95" customHeight="1">
-      <c r="B25" s="11"/>
-      <c r="C25" s="71"/>
-      <c r="D25" s="70"/>
-      <c r="E25" s="153"/>
-      <c r="F25" s="158"/>
-      <c r="G25" s="158"/>
-      <c r="H25" s="158"/>
-      <c r="I25" s="159"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="11"/>
-      <c r="L25" s="72"/>
-      <c r="M25" s="43"/>
-      <c r="N25" s="43"/>
-      <c r="O25" s="55"/>
-    </row>
-    <row r="26" spans="2:16" s="3" customFormat="1" ht="12.75" customHeight="1">
-      <c r="B26" s="35"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="104"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="M24" s="52"/>
+      <c r="N24" s="52"/>
+      <c r="O24" s="66"/>
+    </row>
+    <row r="25" spans="2:16" s="16" customFormat="1" ht="15.95" customHeight="1">
+      <c r="B25" s="64"/>
+      <c r="C25" s="59"/>
+      <c r="D25" s="60"/>
+      <c r="E25" s="58"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="59"/>
+      <c r="H25" s="59"/>
+      <c r="I25" s="60"/>
+      <c r="J25" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="K25" s="40"/>
+      <c r="L25" s="41"/>
+      <c r="M25" s="53"/>
+      <c r="N25" s="53"/>
+      <c r="O25" s="42"/>
+      <c r="P25" s="21"/>
+    </row>
+    <row r="26" spans="2:16" s="16" customFormat="1" ht="12">
+      <c r="B26" s="104" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="105"/>
+      <c r="D26" s="106"/>
+      <c r="E26" s="148"/>
       <c r="F26" s="105"/>
       <c r="G26" s="105"/>
       <c r="H26" s="105"/>
       <c r="I26" s="106"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="12"/>
-      <c r="L26" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="M26" s="52"/>
-      <c r="N26" s="52"/>
+      <c r="J26" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="K26" s="40"/>
+      <c r="L26" s="41"/>
+      <c r="M26" s="53"/>
+      <c r="N26" s="53"/>
       <c r="O26" s="42"/>
     </row>
-    <row r="27" spans="2:16" s="16" customFormat="1" ht="15.95" customHeight="1">
-      <c r="B27" s="68"/>
-      <c r="C27" s="63"/>
-      <c r="D27" s="64"/>
-      <c r="E27" s="62"/>
-      <c r="F27" s="63"/>
-      <c r="G27" s="63"/>
-      <c r="H27" s="63"/>
-      <c r="I27" s="64"/>
+    <row r="27" spans="2:16" s="16" customFormat="1" ht="12">
+      <c r="B27" s="65"/>
+      <c r="C27" s="62"/>
+      <c r="D27" s="63"/>
+      <c r="E27" s="61"/>
+      <c r="F27" s="62"/>
+      <c r="G27" s="62"/>
+      <c r="H27" s="62"/>
+      <c r="I27" s="63"/>
       <c r="J27" s="39" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K27" s="40"/>
       <c r="L27" s="41"/>
       <c r="M27" s="53"/>
       <c r="N27" s="53"/>
       <c r="O27" s="42"/>
-      <c r="P27" s="21"/>
     </row>
     <row r="28" spans="2:16" s="16" customFormat="1" ht="12">
-      <c r="B28" s="107" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" s="108"/>
-      <c r="D28" s="109"/>
-      <c r="E28" s="110"/>
-      <c r="F28" s="111"/>
-      <c r="G28" s="111"/>
-      <c r="H28" s="111"/>
-      <c r="I28" s="112"/>
-      <c r="J28" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="K28" s="40"/>
-      <c r="L28" s="41"/>
-      <c r="M28" s="53"/>
-      <c r="N28" s="53"/>
-      <c r="O28" s="42"/>
+      <c r="B28" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="17"/>
+      <c r="K28" s="17"/>
+      <c r="L28" s="18"/>
+      <c r="M28" s="54"/>
+      <c r="N28" s="54"/>
+      <c r="O28" s="55"/>
     </row>
     <row r="29" spans="2:16" s="16" customFormat="1" ht="12">
-      <c r="B29" s="69"/>
-      <c r="C29" s="66"/>
-      <c r="D29" s="67"/>
-      <c r="E29" s="65"/>
-      <c r="F29" s="66"/>
-      <c r="G29" s="66"/>
-      <c r="H29" s="66"/>
-      <c r="I29" s="67"/>
-      <c r="J29" s="39" t="s">
-        <v>32</v>
-      </c>
-      <c r="K29" s="40"/>
-      <c r="L29" s="41"/>
-      <c r="M29" s="53"/>
-      <c r="N29" s="53"/>
-      <c r="O29" s="42"/>
-    </row>
-    <row r="30" spans="2:16" s="16" customFormat="1" ht="12">
-      <c r="B30" s="36" t="s">
-        <v>33</v>
-      </c>
+      <c r="B29" s="37"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17"/>
+      <c r="J29" s="22"/>
+      <c r="K29" s="22"/>
+      <c r="L29" s="18"/>
+      <c r="M29" s="54"/>
+      <c r="N29" s="54"/>
+      <c r="O29" s="55"/>
+    </row>
+    <row r="30" spans="2:16" s="7" customFormat="1" ht="15" customHeight="1">
+      <c r="B30" s="37"/>
       <c r="C30" s="17"/>
       <c r="D30" s="17"/>
       <c r="E30" s="17"/>
@@ -2395,201 +2375,105 @@
       <c r="I30" s="17"/>
       <c r="J30" s="17"/>
       <c r="K30" s="17"/>
-      <c r="L30" s="18"/>
-      <c r="M30" s="54"/>
-      <c r="N30" s="54"/>
-      <c r="O30" s="55"/>
-    </row>
-    <row r="31" spans="2:16" s="16" customFormat="1" ht="12">
-      <c r="B31" s="37"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="17"/>
-      <c r="I31" s="17"/>
-      <c r="J31" s="22"/>
-      <c r="K31" s="22"/>
-      <c r="L31" s="18"/>
-      <c r="M31" s="54"/>
-      <c r="N31" s="54"/>
-      <c r="O31" s="55"/>
-    </row>
-    <row r="32" spans="2:16" s="16" customFormat="1" ht="12">
-      <c r="B32" s="37"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="17"/>
-      <c r="I32" s="17"/>
-      <c r="J32" s="22"/>
-      <c r="K32" s="22"/>
-      <c r="L32" s="18"/>
-      <c r="M32" s="54"/>
-      <c r="N32" s="54"/>
-      <c r="O32" s="55"/>
-    </row>
-    <row r="33" spans="2:15" s="16" customFormat="1" ht="12">
-      <c r="B33" s="37"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="17"/>
-      <c r="I33" s="17"/>
-      <c r="J33" s="22"/>
-      <c r="K33" s="22"/>
-      <c r="L33" s="18"/>
-      <c r="M33" s="54"/>
-      <c r="N33" s="54"/>
-      <c r="O33" s="55"/>
-    </row>
-    <row r="34" spans="2:15" s="16" customFormat="1" ht="15" customHeight="1">
-      <c r="B34" s="37"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="17"/>
-      <c r="J34" s="22"/>
-      <c r="K34" s="22"/>
-      <c r="L34" s="18"/>
-      <c r="M34" s="54"/>
-      <c r="N34" s="54"/>
-      <c r="O34" s="55"/>
-    </row>
-    <row r="35" spans="2:15" s="16" customFormat="1" ht="12">
-      <c r="B35" s="37"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="17"/>
-      <c r="I35" s="17"/>
-      <c r="J35" s="22"/>
-      <c r="K35" s="22"/>
-      <c r="L35" s="17"/>
-      <c r="M35" s="56"/>
-      <c r="N35" s="56"/>
-      <c r="O35" s="57"/>
-    </row>
-    <row r="36" spans="2:15" s="7" customFormat="1" ht="15" customHeight="1">
-      <c r="B36" s="37"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="17"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="17"/>
-      <c r="H36" s="17"/>
-      <c r="I36" s="17"/>
-      <c r="J36" s="17"/>
-      <c r="K36" s="17"/>
-      <c r="L36" s="19"/>
-      <c r="M36" s="58"/>
-      <c r="N36" s="58"/>
-      <c r="O36" s="59"/>
-    </row>
-    <row r="37" spans="2:15" s="7" customFormat="1" ht="18.75" customHeight="1">
-      <c r="B37" s="38" t="s">
+      <c r="L30" s="19"/>
+      <c r="M30" s="56"/>
+      <c r="N30" s="56"/>
+      <c r="O30" s="57"/>
+    </row>
+    <row r="31" spans="2:16" s="7" customFormat="1" ht="18.75" customHeight="1">
+      <c r="B31" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="C37" s="20"/>
-      <c r="D37" s="26" t="s">
+      <c r="C31" s="20"/>
+      <c r="D31" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="E37" s="26"/>
-      <c r="F37" s="26"/>
-      <c r="G37" s="26"/>
-      <c r="H37" s="27"/>
-      <c r="I37" s="91"/>
-      <c r="J37" s="92"/>
-      <c r="K37" s="93"/>
-      <c r="L37" s="100" t="s">
+      <c r="E31" s="26"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="88"/>
+      <c r="J31" s="89"/>
+      <c r="K31" s="90"/>
+      <c r="L31" s="97" t="s">
         <v>35</v>
       </c>
-      <c r="M37" s="100"/>
-      <c r="N37" s="100"/>
-      <c r="O37" s="101"/>
-    </row>
-    <row r="38" spans="2:15" s="7" customFormat="1" ht="18.75" customHeight="1">
-      <c r="B38" s="79" t="s">
+      <c r="M31" s="97"/>
+      <c r="N31" s="97"/>
+      <c r="O31" s="98"/>
+    </row>
+    <row r="32" spans="2:16" s="7" customFormat="1" ht="18.75" customHeight="1">
+      <c r="B32" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="C38" s="80"/>
-      <c r="D38" s="80"/>
-      <c r="E38" s="80"/>
-      <c r="F38" s="80"/>
-      <c r="G38" s="80"/>
-      <c r="H38" s="81"/>
-      <c r="I38" s="94"/>
-      <c r="J38" s="95"/>
-      <c r="K38" s="96"/>
-      <c r="L38" s="102"/>
-      <c r="M38" s="102"/>
-      <c r="N38" s="102"/>
-      <c r="O38" s="103"/>
-    </row>
-    <row r="39" spans="2:15" s="7" customFormat="1" ht="18.75" customHeight="1">
-      <c r="B39" s="79"/>
-      <c r="C39" s="80"/>
-      <c r="D39" s="80"/>
-      <c r="E39" s="80"/>
-      <c r="F39" s="80"/>
-      <c r="G39" s="80"/>
-      <c r="H39" s="81"/>
-      <c r="I39" s="94"/>
-      <c r="J39" s="95"/>
-      <c r="K39" s="96"/>
-      <c r="L39" s="102"/>
-      <c r="M39" s="102"/>
-      <c r="N39" s="102"/>
-      <c r="O39" s="103"/>
-    </row>
-    <row r="40" spans="2:15" s="7" customFormat="1" ht="11.25">
-      <c r="B40" s="79"/>
-      <c r="C40" s="80"/>
-      <c r="D40" s="80"/>
-      <c r="E40" s="80"/>
-      <c r="F40" s="80"/>
-      <c r="G40" s="80"/>
-      <c r="H40" s="81"/>
-      <c r="I40" s="97"/>
-      <c r="J40" s="98"/>
-      <c r="K40" s="99"/>
-      <c r="L40" s="102"/>
-      <c r="M40" s="102"/>
-      <c r="N40" s="102"/>
-      <c r="O40" s="103"/>
-    </row>
-    <row r="41" spans="2:15" ht="15.75" thickBot="1">
-      <c r="B41" s="82"/>
-      <c r="C41" s="83"/>
-      <c r="D41" s="83"/>
-      <c r="E41" s="83"/>
-      <c r="F41" s="83"/>
-      <c r="G41" s="83"/>
-      <c r="H41" s="84"/>
-      <c r="I41" s="85" t="s">
+      <c r="C32" s="77"/>
+      <c r="D32" s="77"/>
+      <c r="E32" s="77"/>
+      <c r="F32" s="77"/>
+      <c r="G32" s="77"/>
+      <c r="H32" s="78"/>
+      <c r="I32" s="91"/>
+      <c r="J32" s="92"/>
+      <c r="K32" s="93"/>
+      <c r="L32" s="99"/>
+      <c r="M32" s="99"/>
+      <c r="N32" s="99"/>
+      <c r="O32" s="100"/>
+    </row>
+    <row r="33" spans="2:15" s="7" customFormat="1" ht="18.75" customHeight="1">
+      <c r="B33" s="76"/>
+      <c r="C33" s="77"/>
+      <c r="D33" s="77"/>
+      <c r="E33" s="77"/>
+      <c r="F33" s="77"/>
+      <c r="G33" s="77"/>
+      <c r="H33" s="78"/>
+      <c r="I33" s="91"/>
+      <c r="J33" s="92"/>
+      <c r="K33" s="93"/>
+      <c r="L33" s="99"/>
+      <c r="M33" s="99"/>
+      <c r="N33" s="99"/>
+      <c r="O33" s="100"/>
+    </row>
+    <row r="34" spans="2:15" s="7" customFormat="1" ht="11.25">
+      <c r="B34" s="76"/>
+      <c r="C34" s="77"/>
+      <c r="D34" s="77"/>
+      <c r="E34" s="77"/>
+      <c r="F34" s="77"/>
+      <c r="G34" s="77"/>
+      <c r="H34" s="78"/>
+      <c r="I34" s="94"/>
+      <c r="J34" s="95"/>
+      <c r="K34" s="96"/>
+      <c r="L34" s="99"/>
+      <c r="M34" s="99"/>
+      <c r="N34" s="99"/>
+      <c r="O34" s="100"/>
+    </row>
+    <row r="35" spans="2:15" ht="15.75" thickBot="1">
+      <c r="B35" s="79"/>
+      <c r="C35" s="80"/>
+      <c r="D35" s="80"/>
+      <c r="E35" s="80"/>
+      <c r="F35" s="80"/>
+      <c r="G35" s="80"/>
+      <c r="H35" s="81"/>
+      <c r="I35" s="82" t="s">
         <v>36</v>
       </c>
-      <c r="J41" s="86"/>
-      <c r="K41" s="87"/>
-      <c r="L41" s="88" t="s">
+      <c r="J35" s="83"/>
+      <c r="K35" s="84"/>
+      <c r="L35" s="85" t="s">
         <v>37</v>
       </c>
-      <c r="M41" s="89"/>
-      <c r="N41" s="89"/>
-      <c r="O41" s="90"/>
+      <c r="M35" s="86"/>
+      <c r="N35" s="86"/>
+      <c r="O35" s="87"/>
     </row>
   </sheetData>
-  <mergeCells count="41">
+  <mergeCells count="39">
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="D18:H18"/>
     <mergeCell ref="B14:C14"/>
@@ -2597,6 +2481,12 @@
     <mergeCell ref="I14:J14"/>
     <mergeCell ref="B16:H16"/>
     <mergeCell ref="J16:O16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="J17:O17"/>
+    <mergeCell ref="K14:O14"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="I15:O15"/>
     <mergeCell ref="B10:H10"/>
     <mergeCell ref="I10:O10"/>
     <mergeCell ref="B11:O11"/>
@@ -2604,12 +2494,6 @@
     <mergeCell ref="D13:G13"/>
     <mergeCell ref="I13:J13"/>
     <mergeCell ref="K13:O13"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="J17:O17"/>
-    <mergeCell ref="K14:O14"/>
-    <mergeCell ref="C15:H15"/>
-    <mergeCell ref="I15:O15"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="C20:D21"/>
@@ -2618,19 +2502,17 @@
     <mergeCell ref="L20:L21"/>
     <mergeCell ref="O20:O21"/>
     <mergeCell ref="K20:K21"/>
-    <mergeCell ref="B38:H41"/>
-    <mergeCell ref="I41:K41"/>
-    <mergeCell ref="L41:O41"/>
-    <mergeCell ref="I37:K40"/>
-    <mergeCell ref="L37:O37"/>
-    <mergeCell ref="L38:O40"/>
+    <mergeCell ref="B32:H35"/>
+    <mergeCell ref="I35:K35"/>
+    <mergeCell ref="L35:O35"/>
+    <mergeCell ref="I31:K34"/>
+    <mergeCell ref="L31:O31"/>
+    <mergeCell ref="L32:O34"/>
+    <mergeCell ref="E24:I24"/>
+    <mergeCell ref="B26:D26"/>
     <mergeCell ref="E26:I26"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="E28:I28"/>
     <mergeCell ref="E22:I22"/>
     <mergeCell ref="E23:I23"/>
-    <mergeCell ref="E24:I24"/>
-    <mergeCell ref="E25:I25"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J18" r:id="rId1"/>

</xml_diff>